<commit_message>
Updated to reflect files completed and in progress.
git-svn-id: https://subversion.ucar.edu/ncldev/ncarg/branches/NCL_6_0_0@11720 10fe2890-8a40-4696-8b1d-7ccbb19c398e
</commit_message>
<xml_diff>
--- a/ni/src/ncl/NclSrcList.xlsx
+++ b/ni/src/ncl/NclSrcList.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="274">
   <si>
     <r>
       <t xml:space="preserve">Dave</t>
@@ -88,33 +88,39 @@
     <t>AddBuiltIns.c</t>
   </si>
   <si>
+    <t>Reviewed</t>
+  </si>
+  <si>
+    <t>RLB</t>
+  </si>
+  <si>
+    <t>No changes required.</t>
+  </si>
+  <si>
+    <t>AddFileFormats.c</t>
+  </si>
+  <si>
+    <t>AddHLUObjs.c</t>
+  </si>
+  <si>
+    <t>AddIntrinsics.c</t>
+  </si>
+  <si>
+    <t>ApiRecords.h</t>
+  </si>
+  <si>
+    <t>AttSupport.c</t>
+  </si>
+  <si>
+    <t>AttSupport.h</t>
+  </si>
+  <si>
+    <t>BuiltInFuncs.c</t>
+  </si>
+  <si>
     <t>In progress</t>
   </si>
   <si>
-    <t>RLB</t>
-  </si>
-  <si>
-    <t>AddFileFormats.c</t>
-  </si>
-  <si>
-    <t>AddHLUObjs.c</t>
-  </si>
-  <si>
-    <t>AddIntrinsics.c</t>
-  </si>
-  <si>
-    <t>ApiRecords.h</t>
-  </si>
-  <si>
-    <t>AttSupport.c</t>
-  </si>
-  <si>
-    <t>AttSupport.h</t>
-  </si>
-  <si>
-    <t>BuiltInFuncs.c</t>
-  </si>
-  <si>
     <t>Mary</t>
   </si>
   <si>
@@ -130,6 +136,12 @@
     <t>DataSupport.c</t>
   </si>
   <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Minor modifications.</t>
+  </si>
+  <si>
     <t>DataSupport.h</t>
   </si>
   <si>
@@ -139,6 +151,9 @@
     <t>FileSupport.c</t>
   </si>
   <si>
+    <t>Does signature for _NclFileAddVar need to change (see its usage in BuiltInFuncs.c)?</t>
+  </si>
+  <si>
     <t>FileSupport.h</t>
   </si>
   <si>
@@ -350,6 +365,9 @@
   </si>
   <si>
     <t>NclOGR.c</t>
+  </si>
+  <si>
+    <t>Minor mods to interface; OGR does not support &gt;2GB objects/file.</t>
   </si>
   <si>
     <t>NclOneDValCoordData.c</t>
@@ -939,7 +957,7 @@
       <sz val="10"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -955,19 +973,25 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="0000FF00"/>
-        <bgColor rgb="0033CCCC"/>
+        <bgColor rgb="0023FF23"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="0000CCFF"/>
-        <bgColor rgb="0033CCCC"/>
+        <bgColor rgb="0000FFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="00FFFF00"/>
         <bgColor rgb="00FFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0023FF23"/>
+        <bgColor rgb="0000FF00"/>
       </patternFill>
     </fill>
     <fill>
@@ -1015,15 +1039,17 @@
       <protection hidden="false" locked="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="20"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="5" numFmtId="165" xfId="20"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="165" xfId="20"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="4" numFmtId="165" xfId="20"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="20"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="4" fontId="4" numFmtId="165" xfId="20"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="5" fontId="4" numFmtId="165" xfId="20"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="6" fontId="4" numFmtId="165" xfId="20"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="7" fontId="4" numFmtId="165" xfId="20"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -1034,6 +1060,66 @@
     <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
     <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Normal" xfId="20"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0023FF23"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -1082,10 +1168,13 @@
       <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="5">
       <c r="A5" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
@@ -1093,32 +1182,41 @@
       <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="D5" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="6">
       <c r="A6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="D6" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="7">
       <c r="A7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="D7" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="8">
       <c r="A8" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>6</v>
@@ -1126,67 +1224,79 @@
       <c r="C8" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="D8" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="9">
       <c r="A9" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="D9" s="5" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="10">
       <c r="A10" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="D10" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="11">
-      <c r="A11" s="5" t="s">
-        <v>14</v>
+      <c r="A11" s="6" t="s">
+        <v>15</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="12">
-      <c r="A12" s="5" t="s">
-        <v>17</v>
+      <c r="A12" s="6" t="s">
+        <v>19</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="13">
       <c r="A13" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="14">
       <c r="A14" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="D14" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="15">
       <c r="A15" s="4" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>6</v>
@@ -1194,29 +1304,35 @@
       <c r="C15" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="D15" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="16">
-      <c r="A16" s="6" t="s">
-        <v>21</v>
+      <c r="A16" s="7" t="s">
+        <v>25</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="17">
       <c r="A17" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="D17" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="18">
       <c r="A18" s="4" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>7</v>
@@ -1224,7 +1340,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="19">
       <c r="A19" s="4" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>6</v>
@@ -1232,1220 +1348,1232 @@
       <c r="C19" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="D19" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="20">
-      <c r="A20" s="6" t="s">
-        <v>25</v>
+      <c r="A20" s="7" t="s">
+        <v>30</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="21">
-      <c r="A21" s="5" t="s">
-        <v>26</v>
+      <c r="A21" s="6" t="s">
+        <v>31</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="22">
-      <c r="A22" s="5" t="s">
-        <v>27</v>
+      <c r="A22" s="6" t="s">
+        <v>32</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="23">
-      <c r="A23" s="5" t="s">
-        <v>28</v>
+      <c r="A23" s="6" t="s">
+        <v>33</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="24">
-      <c r="A24" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="25">
-      <c r="A25" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="26">
-      <c r="A26" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="27">
-      <c r="A27" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="28">
-      <c r="A28" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="29">
-      <c r="A29" s="1" t="s">
+      <c r="A24" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="30">
-      <c r="A30" s="1" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="25">
+      <c r="A25" s="8" t="s">
         <v>35</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="31">
-      <c r="A31" s="1" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="26">
+      <c r="A26" s="8" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="27">
+      <c r="A27" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="28">
+      <c r="A28" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="29">
+      <c r="A29" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="30">
+      <c r="A30" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="31">
+      <c r="A31" s="8" t="s">
+        <v>41</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="32">
       <c r="A32" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="33">
       <c r="A33" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="34">
       <c r="A34" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="35">
       <c r="A35" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="36">
       <c r="A36" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="37">
       <c r="A37" s="1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="38">
       <c r="A38" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="39">
-      <c r="A39" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="39">
+      <c r="A39" s="8" t="s">
+        <v>49</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="40">
       <c r="A40" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="41">
-      <c r="A41" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="42">
-      <c r="A42" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="43">
-      <c r="A43" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="41">
+      <c r="A41" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="42">
+      <c r="A42" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="43">
+      <c r="A43" s="8" t="s">
+        <v>53</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="44">
       <c r="A44" s="1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="45">
       <c r="A45" s="1" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="46">
       <c r="A46" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="47">
       <c r="A47" s="1" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="48">
       <c r="A48" s="1" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="49">
       <c r="A49" s="1" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="50">
       <c r="A50" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="51">
       <c r="A51" s="1" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="52">
       <c r="A52" s="1" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="53">
       <c r="A53" s="1" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="54">
-      <c r="A54" s="6" t="s">
-        <v>59</v>
+      <c r="A54" s="7" t="s">
+        <v>64</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="55">
-      <c r="A55" s="6" t="s">
-        <v>60</v>
+      <c r="A55" s="7" t="s">
+        <v>65</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="56">
-      <c r="A56" s="6" t="s">
-        <v>61</v>
+      <c r="A56" s="7" t="s">
+        <v>66</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="57">
-      <c r="A57" s="6" t="s">
-        <v>62</v>
+      <c r="A57" s="7" t="s">
+        <v>67</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="58">
-      <c r="A58" s="6" t="s">
-        <v>63</v>
+      <c r="A58" s="7" t="s">
+        <v>68</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="59">
-      <c r="A59" s="6" t="s">
-        <v>64</v>
+      <c r="A59" s="7" t="s">
+        <v>69</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="60">
-      <c r="A60" s="6" t="s">
-        <v>65</v>
+      <c r="A60" s="7" t="s">
+        <v>70</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="61">
-      <c r="A61" s="6" t="s">
-        <v>66</v>
+      <c r="A61" s="7" t="s">
+        <v>71</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="62">
-      <c r="A62" s="6" t="s">
-        <v>67</v>
+      <c r="A62" s="7" t="s">
+        <v>72</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="63">
-      <c r="A63" s="6" t="s">
-        <v>68</v>
+      <c r="A63" s="7" t="s">
+        <v>73</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="64">
-      <c r="A64" s="6" t="s">
-        <v>69</v>
+      <c r="A64" s="7" t="s">
+        <v>74</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="65">
-      <c r="A65" s="6" t="s">
-        <v>70</v>
+      <c r="A65" s="7" t="s">
+        <v>75</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="66">
-      <c r="A66" s="6" t="s">
-        <v>71</v>
+      <c r="A66" s="7" t="s">
+        <v>76</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="67">
-      <c r="A67" s="6" t="s">
-        <v>72</v>
+      <c r="A67" s="7" t="s">
+        <v>77</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="68">
-      <c r="A68" s="7" t="s">
-        <v>73</v>
+      <c r="A68" s="9" t="s">
+        <v>78</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="69">
-      <c r="A69" s="7" t="s">
-        <v>74</v>
+      <c r="A69" s="9" t="s">
+        <v>79</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="70">
-      <c r="A70" s="7" t="s">
-        <v>75</v>
+      <c r="A70" s="9" t="s">
+        <v>80</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="71">
-      <c r="A71" s="6" t="s">
-        <v>76</v>
+      <c r="A71" s="7" t="s">
+        <v>81</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="72">
-      <c r="A72" s="6" t="s">
-        <v>77</v>
+      <c r="A72" s="7" t="s">
+        <v>82</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="73">
-      <c r="A73" s="6" t="s">
-        <v>78</v>
+      <c r="A73" s="7" t="s">
+        <v>83</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="74">
-      <c r="A74" s="6" t="s">
-        <v>79</v>
+      <c r="A74" s="7" t="s">
+        <v>84</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="75">
-      <c r="A75" s="6" t="s">
-        <v>80</v>
+      <c r="A75" s="7" t="s">
+        <v>85</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="76">
-      <c r="A76" s="6" t="s">
-        <v>81</v>
+      <c r="A76" s="7" t="s">
+        <v>86</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="77">
-      <c r="A77" s="6" t="s">
-        <v>82</v>
+      <c r="A77" s="7" t="s">
+        <v>87</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="78">
-      <c r="A78" s="6" t="s">
-        <v>83</v>
+      <c r="A78" s="7" t="s">
+        <v>88</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="79">
-      <c r="A79" s="6" t="s">
-        <v>84</v>
+      <c r="A79" s="7" t="s">
+        <v>89</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="80">
-      <c r="A80" s="6" t="s">
-        <v>85</v>
+      <c r="A80" s="7" t="s">
+        <v>90</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="81">
-      <c r="A81" s="6" t="s">
-        <v>86</v>
+      <c r="A81" s="7" t="s">
+        <v>91</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="82">
-      <c r="A82" s="6" t="s">
-        <v>87</v>
+      <c r="A82" s="7" t="s">
+        <v>92</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="83">
-      <c r="A83" s="6" t="s">
-        <v>88</v>
+      <c r="A83" s="7" t="s">
+        <v>93</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="84">
-      <c r="A84" s="6" t="s">
-        <v>89</v>
+      <c r="A84" s="7" t="s">
+        <v>94</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="85">
-      <c r="A85" s="6" t="s">
-        <v>90</v>
+      <c r="A85" s="7" t="s">
+        <v>95</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="86">
-      <c r="A86" s="6" t="s">
-        <v>91</v>
+      <c r="A86" s="7" t="s">
+        <v>96</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="87">
-      <c r="A87" s="6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="88">
+      <c r="A87" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="88">
       <c r="A88" s="4" t="s">
-        <v>93</v>
+        <v>98</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>99</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="89">
       <c r="A89" s="1" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="90">
       <c r="A90" s="1" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="91">
-      <c r="A91" s="7" t="s">
-        <v>96</v>
+      <c r="A91" s="9" t="s">
+        <v>102</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="92">
-      <c r="A92" s="7" t="s">
-        <v>97</v>
+      <c r="A92" s="9" t="s">
+        <v>103</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="93">
-      <c r="A93" s="7" t="s">
-        <v>98</v>
+      <c r="A93" s="9" t="s">
+        <v>104</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="94">
-      <c r="A94" s="7" t="s">
-        <v>99</v>
+      <c r="A94" s="9" t="s">
+        <v>105</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="95">
-      <c r="A95" s="7" t="s">
-        <v>100</v>
+      <c r="A95" s="9" t="s">
+        <v>106</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="96">
-      <c r="A96" s="7" t="s">
-        <v>101</v>
+      <c r="A96" s="9" t="s">
+        <v>107</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="97">
-      <c r="A97" s="7" t="s">
-        <v>102</v>
+      <c r="A97" s="9" t="s">
+        <v>108</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="98">
-      <c r="A98" s="7" t="s">
-        <v>103</v>
+      <c r="A98" s="9" t="s">
+        <v>109</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="99">
-      <c r="A99" s="7" t="s">
-        <v>104</v>
+      <c r="A99" s="9" t="s">
+        <v>110</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="100">
-      <c r="A100" s="7" t="s">
-        <v>105</v>
+      <c r="A100" s="9" t="s">
+        <v>111</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="101">
-      <c r="A101" s="7" t="s">
-        <v>106</v>
+      <c r="A101" s="9" t="s">
+        <v>112</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="102">
-      <c r="A102" s="7" t="s">
-        <v>107</v>
+      <c r="A102" s="9" t="s">
+        <v>113</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="103">
-      <c r="A103" s="7" t="s">
-        <v>108</v>
+      <c r="A103" s="9" t="s">
+        <v>114</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="104">
-      <c r="A104" s="7" t="s">
-        <v>109</v>
+      <c r="A104" s="9" t="s">
+        <v>115</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="105">
-      <c r="A105" s="7" t="s">
-        <v>110</v>
+      <c r="A105" s="9" t="s">
+        <v>116</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="106">
-      <c r="A106" s="7" t="s">
-        <v>111</v>
+      <c r="A106" s="9" t="s">
+        <v>117</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="107">
-      <c r="A107" s="7" t="s">
-        <v>112</v>
+      <c r="A107" s="9" t="s">
+        <v>118</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="108">
-      <c r="A108" s="7" t="s">
-        <v>113</v>
+      <c r="A108" s="9" t="s">
+        <v>119</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="109">
-      <c r="A109" s="7" t="s">
-        <v>114</v>
+      <c r="A109" s="9" t="s">
+        <v>120</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="110">
-      <c r="A110" s="7" t="s">
-        <v>115</v>
+      <c r="A110" s="9" t="s">
+        <v>121</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="111">
-      <c r="A111" s="7" t="s">
-        <v>116</v>
+      <c r="A111" s="9" t="s">
+        <v>122</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="112">
-      <c r="A112" s="7" t="s">
-        <v>117</v>
+      <c r="A112" s="9" t="s">
+        <v>123</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="113">
-      <c r="A113" s="7" t="s">
-        <v>118</v>
+      <c r="A113" s="9" t="s">
+        <v>124</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="114">
-      <c r="A114" s="7" t="s">
-        <v>119</v>
+      <c r="A114" s="9" t="s">
+        <v>125</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="115">
-      <c r="A115" s="7" t="s">
-        <v>120</v>
+      <c r="A115" s="9" t="s">
+        <v>126</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="116">
-      <c r="A116" s="7" t="s">
-        <v>121</v>
+      <c r="A116" s="9" t="s">
+        <v>127</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="117">
-      <c r="A117" s="7" t="s">
-        <v>122</v>
+      <c r="A117" s="9" t="s">
+        <v>128</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="118">
-      <c r="A118" s="6" t="s">
-        <v>123</v>
+      <c r="A118" s="7" t="s">
+        <v>129</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="119">
-      <c r="A119" s="6" t="s">
-        <v>124</v>
+      <c r="A119" s="7" t="s">
+        <v>130</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="120">
       <c r="A120" s="1" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="121">
       <c r="A121" s="1" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="122">
       <c r="A122" s="1" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="123">
       <c r="A123" s="1" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="124">
       <c r="A124" s="1" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="125">
       <c r="A125" s="1" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="126">
       <c r="A126" s="1" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="127">
-      <c r="A127" s="6" t="s">
-        <v>132</v>
+      <c r="A127" s="7" t="s">
+        <v>138</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="128">
-      <c r="A128" s="6" t="s">
-        <v>133</v>
+      <c r="A128" s="7" t="s">
+        <v>139</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="129">
-      <c r="A129" s="6" t="s">
-        <v>134</v>
+      <c r="A129" s="7" t="s">
+        <v>140</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="130">
-      <c r="A130" s="6" t="s">
-        <v>135</v>
+      <c r="A130" s="7" t="s">
+        <v>141</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="131">
-      <c r="A131" s="6" t="s">
-        <v>136</v>
+      <c r="A131" s="7" t="s">
+        <v>142</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="132">
-      <c r="A132" s="6" t="s">
-        <v>137</v>
+      <c r="A132" s="7" t="s">
+        <v>143</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="133">
-      <c r="A133" s="6" t="s">
-        <v>138</v>
+      <c r="A133" s="7" t="s">
+        <v>144</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="134">
-      <c r="A134" s="6" t="s">
-        <v>139</v>
+      <c r="A134" s="7" t="s">
+        <v>145</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="135">
-      <c r="A135" s="6" t="s">
-        <v>140</v>
+      <c r="A135" s="7" t="s">
+        <v>146</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="136">
-      <c r="A136" s="6" t="s">
-        <v>141</v>
+      <c r="A136" s="7" t="s">
+        <v>147</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="137">
-      <c r="A137" s="6" t="s">
-        <v>142</v>
+      <c r="A137" s="7" t="s">
+        <v>148</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="138">
-      <c r="A138" s="6" t="s">
-        <v>143</v>
+      <c r="A138" s="7" t="s">
+        <v>149</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="139">
-      <c r="A139" s="6" t="s">
-        <v>144</v>
+      <c r="A139" s="7" t="s">
+        <v>150</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="140">
-      <c r="A140" s="6" t="s">
-        <v>145</v>
+      <c r="A140" s="7" t="s">
+        <v>151</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="141">
-      <c r="A141" s="6" t="s">
-        <v>146</v>
+      <c r="A141" s="7" t="s">
+        <v>152</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="142">
-      <c r="A142" s="6" t="s">
-        <v>147</v>
+      <c r="A142" s="7" t="s">
+        <v>153</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="143">
-      <c r="A143" s="6" t="s">
-        <v>148</v>
+      <c r="A143" s="7" t="s">
+        <v>154</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="144">
-      <c r="A144" s="6" t="s">
-        <v>149</v>
+      <c r="A144" s="7" t="s">
+        <v>155</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="145">
-      <c r="A145" s="6" t="s">
-        <v>150</v>
+      <c r="A145" s="7" t="s">
+        <v>156</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="146">
-      <c r="A146" s="6" t="s">
-        <v>151</v>
+      <c r="A146" s="7" t="s">
+        <v>157</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="147">
-      <c r="A147" s="6" t="s">
-        <v>152</v>
+      <c r="A147" s="7" t="s">
+        <v>158</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="148">
-      <c r="A148" s="6" t="s">
-        <v>153</v>
+      <c r="A148" s="7" t="s">
+        <v>159</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="149">
-      <c r="A149" s="6" t="s">
-        <v>154</v>
+      <c r="A149" s="7" t="s">
+        <v>160</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="150">
-      <c r="A150" s="6" t="s">
-        <v>155</v>
+      <c r="A150" s="7" t="s">
+        <v>161</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="151">
-      <c r="A151" s="6" t="s">
-        <v>156</v>
+      <c r="A151" s="7" t="s">
+        <v>162</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="152">
       <c r="A152" s="1" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="153">
       <c r="A153" s="1" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="154">
       <c r="A154" s="1" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="155">
       <c r="A155" s="1" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="156">
       <c r="A156" s="1" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="157">
       <c r="A157" s="1" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="158">
       <c r="A158" s="1" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="159">
       <c r="A159" s="1" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="160">
       <c r="A160" s="1" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="161">
       <c r="A161" s="1" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="162">
       <c r="A162" s="1" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="163">
       <c r="A163" s="1" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="164">
       <c r="A164" s="1" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="165">
       <c r="A165" s="1" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="166">
       <c r="A166" s="1" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="167">
       <c r="A167" s="1" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="168">
       <c r="A168" s="1" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="169">
       <c r="A169" s="1" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="170">
       <c r="A170" s="1" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="171">
       <c r="A171" s="1" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="172">
       <c r="A172" s="1" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="173">
       <c r="A173" s="1" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="174">
       <c r="A174" s="1" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="175">
       <c r="A175" s="1" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="176">
       <c r="A176" s="1" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="177">
       <c r="A177" s="1" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="178">
       <c r="A178" s="1" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="179">
       <c r="A179" s="1" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="180">
       <c r="A180" s="1" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="181">
       <c r="A181" s="1" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="182">
       <c r="A182" s="1" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="183">
       <c r="A183" s="1" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="184">
       <c r="A184" s="1" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="185">
       <c r="A185" s="1" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="186">
       <c r="A186" s="1" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="187">
       <c r="A187" s="1" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="188">
       <c r="A188" s="1" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="189">
       <c r="A189" s="1" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="190">
       <c r="A190" s="1" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="191">
       <c r="A191" s="1" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="192">
       <c r="A192" s="1" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="193">
       <c r="A193" s="1" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="194">
       <c r="A194" s="1" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="195">
       <c r="A195" s="1" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="196">
       <c r="A196" s="1" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="197">
       <c r="A197" s="1" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="198">
       <c r="A198" s="1" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="199">
       <c r="A199" s="1" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="200">
       <c r="A200" s="1" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="201">
       <c r="A201" s="1" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="202">
       <c r="A202" s="1" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="203">
       <c r="A203" s="1" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="204">
       <c r="A204" s="1" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="205">
       <c r="A205" s="1" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="206">
       <c r="A206" s="1" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="207">
       <c r="A207" s="1" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="208">
       <c r="A208" s="1" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="209">
       <c r="A209" s="1" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="210">
       <c r="A210" s="1" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="211">
       <c r="A211" s="1" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="212">
       <c r="A212" s="1" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="213">
       <c r="A213" s="1" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="214">
       <c r="A214" s="1" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="215">
       <c r="A215" s="1" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="216">
       <c r="A216" s="1" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="217">
       <c r="A217" s="1" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="218">
       <c r="A218" s="1" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="219">
       <c r="A219" s="1" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="220">
       <c r="A220" s="1" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="221">
       <c r="A221" s="1" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="222">
       <c r="A222" s="1" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="223">
       <c r="A223" s="1" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="224">
       <c r="A224" s="1" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="225">
       <c r="A225" s="1" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="226">
       <c r="A226" s="1" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="227">
       <c r="A227" s="1" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="228">
       <c r="A228" s="1" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="229">
       <c r="A229" s="1" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="230">
       <c r="A230" s="1" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="231">
       <c r="A231" s="1" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="232">
       <c r="A232" s="1" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="233">
       <c r="A233" s="1" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="234">
-      <c r="A234" s="6" t="s">
-        <v>239</v>
+      <c r="A234" s="7" t="s">
+        <v>245</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="235">
-      <c r="A235" s="6" t="s">
-        <v>240</v>
+      <c r="A235" s="7" t="s">
+        <v>246</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="236">
       <c r="A236" s="1" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="237">
       <c r="A237" s="1" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="238">
       <c r="A238" s="1" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="239">
       <c r="A239" s="1" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="240">
       <c r="A240" s="1" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="241">
       <c r="A241" s="1" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="242">
       <c r="A242" s="1" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="243">
-      <c r="A243" s="6" t="s">
-        <v>248</v>
+      <c r="A243" s="7" t="s">
+        <v>254</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="244">
-      <c r="A244" s="6" t="s">
-        <v>249</v>
+      <c r="A244" s="7" t="s">
+        <v>255</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="245">
-      <c r="A245" s="6" t="s">
-        <v>250</v>
+      <c r="A245" s="7" t="s">
+        <v>256</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="246">
-      <c r="A246" s="6" t="s">
-        <v>251</v>
+      <c r="A246" s="7" t="s">
+        <v>257</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="247">
-      <c r="A247" s="6" t="s">
-        <v>252</v>
+      <c r="A247" s="7" t="s">
+        <v>258</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="248">
-      <c r="A248" s="6" t="s">
-        <v>253</v>
+      <c r="A248" s="7" t="s">
+        <v>259</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="249">
-      <c r="A249" s="6" t="s">
-        <v>254</v>
+      <c r="A249" s="7" t="s">
+        <v>260</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="250">
-      <c r="A250" s="6" t="s">
-        <v>255</v>
+      <c r="A250" s="7" t="s">
+        <v>261</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="251">
       <c r="A251" s="1" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="252">
       <c r="A252" s="1" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="253">
-      <c r="A253" s="7" t="s">
-        <v>258</v>
+      <c r="A253" s="9" t="s">
+        <v>264</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="254">
-      <c r="A254" s="7" t="s">
-        <v>259</v>
+      <c r="A254" s="9" t="s">
+        <v>265</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="255">
-      <c r="A255" s="7" t="s">
-        <v>260</v>
+      <c r="A255" s="9" t="s">
+        <v>266</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="256">
-      <c r="A256" s="7" t="s">
-        <v>261</v>
+      <c r="A256" s="9" t="s">
+        <v>267</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="257">
-      <c r="A257" s="7" t="s">
-        <v>262</v>
+      <c r="A257" s="9" t="s">
+        <v>268</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="258">
-      <c r="A258" s="7" t="s">
-        <v>263</v>
+      <c r="A258" s="9" t="s">
+        <v>269</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="259">
-      <c r="A259" s="7" t="s">
-        <v>264</v>
+      <c r="A259" s="9" t="s">
+        <v>270</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="260">
-      <c r="A260" s="7" t="s">
-        <v>265</v>
+      <c r="A260" s="9" t="s">
+        <v>271</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="261">
-      <c r="A261" s="7" t="s">
-        <v>266</v>
+      <c r="A261" s="9" t="s">
+        <v>272</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="262">
       <c r="A262" s="1" t="s">
-        <v>267</v>
+        <v>273</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update status and new assignments.
git-svn-id: https://subversion.ucar.edu/ncldev/ncarg/branches/NCL_6_0_0@11726 10fe2890-8a40-4696-8b1d-7ccbb19c398e
</commit_message>
<xml_diff>
--- a/ni/src/ncl/NclSrcList.xlsx
+++ b/ni/src/ncl/NclSrcList.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="280">
   <si>
     <r>
       <t xml:space="preserve">Dave</t>
@@ -252,9 +252,15 @@
     <t>NclAtt.c</t>
   </si>
   <si>
+    <t>Patched </t>
+  </si>
+  <si>
     <t>NclAtt.h</t>
   </si>
   <si>
+    <t>Number of attributes never &gt;2GB?</t>
+  </si>
+  <si>
     <t>NclBuiltInSupport.h</t>
   </si>
   <si>
@@ -282,6 +288,9 @@
     <t>NclData.h</t>
   </si>
   <si>
+    <t>Does NclSelectionRecord.n_entries need to be ng_size_t?  --RLB</t>
+  </si>
+  <si>
     <t>NclDataDefs.h</t>
   </si>
   <si>
@@ -384,13 +393,13 @@
     <t>NclOGR.c</t>
   </si>
   <si>
-    <t>Done</t>
-  </si>
-  <si>
     <t>Minor mods to interface; OGR does not support &gt;2GB objects/file.</t>
   </si>
   <si>
     <t>NclOneDValCoordData.c</t>
+  </si>
+  <si>
+    <t>Minor mods to local vars that iterate over a range of ng_size_t</t>
   </si>
   <si>
     <t>NclOneDValCoordData.h</t>
@@ -1065,7 +1074,7 @@
       <protection hidden="false" locked="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="20"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="5" numFmtId="165" xfId="20"/>
@@ -1075,6 +1084,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="4" fontId="4" numFmtId="165" xfId="20"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="5" fontId="4" numFmtId="165" xfId="20"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="6" fontId="4" numFmtId="165" xfId="20"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="20"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="7" fontId="4" numFmtId="165" xfId="20"/>
   </cellXfs>
   <cellStyles count="7">
@@ -1599,1104 +1609,1197 @@
       <c r="A44" s="4" t="s">
         <v>56</v>
       </c>
+      <c r="B44" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="45">
       <c r="A45" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>59</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="46">
       <c r="A46" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="47">
       <c r="A47" s="4" t="s">
-        <v>59</v>
+        <v>61</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="48">
-      <c r="A48" s="4" t="s">
-        <v>60</v>
+      <c r="A48" s="9" t="s">
+        <v>62</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="49">
-      <c r="A49" s="4" t="s">
-        <v>61</v>
+      <c r="A49" s="9" t="s">
+        <v>63</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="50">
       <c r="A50" s="4" t="s">
-        <v>62</v>
+        <v>64</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="51">
       <c r="A51" s="4" t="s">
-        <v>63</v>
+        <v>65</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="52">
       <c r="A52" s="4" t="s">
-        <v>64</v>
+        <v>66</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="53">
       <c r="A53" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="54">
+        <v>67</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="54">
       <c r="A54" s="7" t="s">
-        <v>66</v>
+        <v>68</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>69</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="55">
       <c r="A55" s="7" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="56">
       <c r="A56" s="7" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="57">
       <c r="A57" s="7" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="58">
       <c r="A58" s="7" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="59">
       <c r="A59" s="7" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="60">
       <c r="A60" s="7" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="61">
       <c r="A61" s="7" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="62">
       <c r="A62" s="7" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="63">
       <c r="A63" s="7" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="64">
       <c r="A64" s="7" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="65">
       <c r="A65" s="7" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="66">
       <c r="A66" s="7" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="67">
       <c r="A67" s="7" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="68">
-      <c r="A68" s="9" t="s">
-        <v>80</v>
+      <c r="A68" s="10" t="s">
+        <v>83</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="69">
-      <c r="A69" s="9" t="s">
-        <v>81</v>
+      <c r="A69" s="10" t="s">
+        <v>84</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="70">
-      <c r="A70" s="9" t="s">
-        <v>82</v>
+      <c r="A70" s="10" t="s">
+        <v>85</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="71">
       <c r="A71" s="7" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="72">
       <c r="A72" s="7" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="73">
       <c r="A73" s="7" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="74">
       <c r="A74" s="7" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="75">
       <c r="A75" s="7" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="76">
       <c r="A76" s="7" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="77">
       <c r="A77" s="7" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="78">
       <c r="A78" s="7" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="79">
       <c r="A79" s="7" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="80">
       <c r="A80" s="7" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="81">
       <c r="A81" s="7" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="82">
       <c r="A82" s="7" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="83">
       <c r="A83" s="7" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="84">
       <c r="A84" s="7" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="85">
       <c r="A85" s="7" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="86">
       <c r="A86" s="7" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="87">
       <c r="A87" s="7" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="88">
       <c r="A88" s="4" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>101</v>
+        <v>22</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="89">
-      <c r="A89" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="90">
-      <c r="A90" s="1" t="s">
         <v>104</v>
       </c>
     </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="89">
+      <c r="A89" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="90">
+      <c r="A90" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="91">
-      <c r="A91" s="9" t="s">
-        <v>105</v>
+      <c r="A91" s="10" t="s">
+        <v>108</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="92">
-      <c r="A92" s="9" t="s">
-        <v>106</v>
+      <c r="A92" s="10" t="s">
+        <v>109</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="93">
-      <c r="A93" s="9" t="s">
-        <v>107</v>
+      <c r="A93" s="10" t="s">
+        <v>110</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="94">
-      <c r="A94" s="9" t="s">
-        <v>108</v>
+      <c r="A94" s="10" t="s">
+        <v>111</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="95">
-      <c r="A95" s="9" t="s">
-        <v>109</v>
+      <c r="A95" s="10" t="s">
+        <v>112</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="96">
-      <c r="A96" s="9" t="s">
-        <v>110</v>
+      <c r="A96" s="10" t="s">
+        <v>113</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="97">
-      <c r="A97" s="9" t="s">
-        <v>111</v>
+      <c r="A97" s="10" t="s">
+        <v>114</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="98">
-      <c r="A98" s="9" t="s">
-        <v>112</v>
+      <c r="A98" s="10" t="s">
+        <v>115</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="99">
-      <c r="A99" s="9" t="s">
-        <v>113</v>
+      <c r="A99" s="10" t="s">
+        <v>116</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="100">
-      <c r="A100" s="9" t="s">
-        <v>114</v>
+      <c r="A100" s="10" t="s">
+        <v>117</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="101">
-      <c r="A101" s="9" t="s">
-        <v>115</v>
+      <c r="A101" s="10" t="s">
+        <v>118</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="102">
-      <c r="A102" s="9" t="s">
-        <v>116</v>
+      <c r="A102" s="10" t="s">
+        <v>119</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="103">
-      <c r="A103" s="9" t="s">
-        <v>117</v>
+      <c r="A103" s="10" t="s">
+        <v>120</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="104">
-      <c r="A104" s="9" t="s">
-        <v>118</v>
+      <c r="A104" s="10" t="s">
+        <v>121</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="105">
-      <c r="A105" s="9" t="s">
-        <v>119</v>
+      <c r="A105" s="10" t="s">
+        <v>122</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="106">
-      <c r="A106" s="9" t="s">
-        <v>120</v>
+      <c r="A106" s="10" t="s">
+        <v>123</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="107">
-      <c r="A107" s="9" t="s">
-        <v>121</v>
+      <c r="A107" s="10" t="s">
+        <v>124</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="108">
-      <c r="A108" s="9" t="s">
-        <v>122</v>
+      <c r="A108" s="10" t="s">
+        <v>125</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="109">
-      <c r="A109" s="9" t="s">
-        <v>123</v>
+      <c r="A109" s="10" t="s">
+        <v>126</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="110">
-      <c r="A110" s="9" t="s">
-        <v>124</v>
+      <c r="A110" s="10" t="s">
+        <v>127</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="111">
-      <c r="A111" s="9" t="s">
-        <v>125</v>
+      <c r="A111" s="10" t="s">
+        <v>128</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="112">
-      <c r="A112" s="9" t="s">
-        <v>126</v>
+      <c r="A112" s="10" t="s">
+        <v>129</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="113">
-      <c r="A113" s="9" t="s">
-        <v>127</v>
+      <c r="A113" s="10" t="s">
+        <v>130</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="114">
-      <c r="A114" s="9" t="s">
-        <v>128</v>
+      <c r="A114" s="10" t="s">
+        <v>131</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="115">
-      <c r="A115" s="9" t="s">
-        <v>129</v>
+      <c r="A115" s="10" t="s">
+        <v>132</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="116">
-      <c r="A116" s="9" t="s">
-        <v>130</v>
+      <c r="A116" s="10" t="s">
+        <v>133</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="117">
-      <c r="A117" s="9" t="s">
-        <v>131</v>
+      <c r="A117" s="10" t="s">
+        <v>134</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="118">
       <c r="A118" s="7" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="119">
       <c r="A119" s="7" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="120">
-      <c r="A120" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="121">
-      <c r="A121" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="122">
-      <c r="A122" s="1" t="s">
         <v>136</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="123">
-      <c r="A123" s="1" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="120">
+      <c r="A120" s="4" t="s">
         <v>137</v>
       </c>
     </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="121">
+      <c r="A121" s="4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="122">
+      <c r="A122" s="4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="123">
+      <c r="A123" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="124">
-      <c r="A124" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="125">
-      <c r="A125" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="126">
-      <c r="A126" s="1" t="s">
-        <v>140</v>
+      <c r="A124" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="125">
+      <c r="A125" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="126">
+      <c r="A126" s="4" t="s">
+        <v>143</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="127">
       <c r="A127" s="7" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="128">
       <c r="A128" s="7" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="129">
       <c r="A129" s="7" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="130">
       <c r="A130" s="7" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="131">
       <c r="A131" s="7" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="132">
       <c r="A132" s="7" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="133">
       <c r="A133" s="7" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="134">
       <c r="A134" s="7" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="135">
       <c r="A135" s="7" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="136">
       <c r="A136" s="7" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="137">
       <c r="A137" s="7" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="138">
       <c r="A138" s="7" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="139">
       <c r="A139" s="7" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="140">
       <c r="A140" s="7" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="141">
       <c r="A141" s="7" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="142">
       <c r="A142" s="7" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="143">
       <c r="A143" s="7" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="144">
       <c r="A144" s="7" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="145">
       <c r="A145" s="7" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="146">
       <c r="A146" s="7" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="147">
       <c r="A147" s="7" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="148">
       <c r="A148" s="7" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="149">
       <c r="A149" s="7" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="150">
       <c r="A150" s="7" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="151">
       <c r="A151" s="7" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="152">
-      <c r="A152" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="153">
-      <c r="A153" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="152">
+      <c r="A152" s="4" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="153">
+      <c r="A153" s="4" t="s">
+        <v>170</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="154">
       <c r="A154" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="155">
-      <c r="A155" s="1" t="s">
-        <v>169</v>
+        <v>171</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="155">
+      <c r="A155" s="4" t="s">
+        <v>172</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="156">
       <c r="A156" s="1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="157">
-      <c r="A157" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="158">
-      <c r="A158" s="1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="159">
-      <c r="A159" s="1" t="s">
         <v>173</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="160">
-      <c r="A160" s="1" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="157">
+      <c r="A157" s="4" t="s">
         <v>174</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="158">
+      <c r="A158" s="4" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="159">
+      <c r="A159" s="4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="160">
+      <c r="A160" s="4" t="s">
+        <v>177</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="161">
       <c r="A161" s="1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="162">
-      <c r="A162" s="1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="163">
-      <c r="A163" s="1" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="164">
-      <c r="A164" s="1" t="s">
         <v>178</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="162">
+      <c r="A162" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="163">
+      <c r="A163" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="164">
+      <c r="A164" s="4" t="s">
+        <v>181</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="165">
       <c r="A165" s="1" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="166">
       <c r="A166" s="1" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="167">
       <c r="A167" s="1" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="168">
       <c r="A168" s="1" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="169">
       <c r="A169" s="1" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="170">
       <c r="A170" s="1" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="171">
       <c r="A171" s="1" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="172">
       <c r="A172" s="1" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="173">
       <c r="A173" s="1" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="174">
       <c r="A174" s="1" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="175">
       <c r="A175" s="1" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="176">
       <c r="A176" s="1" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="177">
       <c r="A177" s="1" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="178">
       <c r="A178" s="1" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="179">
       <c r="A179" s="1" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="180">
       <c r="A180" s="1" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="181">
       <c r="A181" s="1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="182">
       <c r="A182" s="1" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="183">
       <c r="A183" s="1" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="184">
       <c r="A184" s="1" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="185">
       <c r="A185" s="1" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="186">
       <c r="A186" s="1" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="187">
       <c r="A187" s="1" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="188">
       <c r="A188" s="1" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="189">
       <c r="A189" s="1" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="190">
       <c r="A190" s="1" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="191">
       <c r="A191" s="1" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="192">
       <c r="A192" s="1" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="193">
       <c r="A193" s="1" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="194">
       <c r="A194" s="1" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="195">
       <c r="A195" s="1" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="196">
       <c r="A196" s="1" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="197">
       <c r="A197" s="1" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="198">
       <c r="A198" s="1" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="199">
       <c r="A199" s="1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="200">
-      <c r="A200" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="201">
-      <c r="A201" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="202">
-      <c r="A202" s="1" t="s">
         <v>216</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="200">
+      <c r="A200" s="4" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="201">
+      <c r="A201" s="4" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="202">
+      <c r="A202" s="4" t="s">
+        <v>219</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="203">
       <c r="A203" s="1" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="204">
       <c r="A204" s="1" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="205">
       <c r="A205" s="1" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="206">
       <c r="A206" s="1" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="207">
       <c r="A207" s="1" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="208">
       <c r="A208" s="1" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="209">
       <c r="A209" s="1" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="210">
       <c r="A210" s="1" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="211">
       <c r="A211" s="1" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="212">
       <c r="A212" s="1" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="213">
       <c r="A213" s="1" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="214">
       <c r="A214" s="1" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="215">
       <c r="A215" s="1" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="216">
-      <c r="A216" s="1" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="217">
-      <c r="A217" s="1" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="218">
-      <c r="A218" s="1" t="s">
         <v>232</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="216">
+      <c r="A216" s="4" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="217">
+      <c r="A217" s="4" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="218">
+      <c r="A218" s="4" t="s">
+        <v>235</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="219">
       <c r="A219" s="1" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="220">
       <c r="A220" s="1" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="221">
       <c r="A221" s="1" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="222">
       <c r="A222" s="1" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="223">
       <c r="A223" s="1" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="224">
       <c r="A224" s="1" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="225">
       <c r="A225" s="1" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="226">
       <c r="A226" s="1" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="227">
       <c r="A227" s="1" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="228">
       <c r="A228" s="1" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="229">
       <c r="A229" s="1" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="230">
       <c r="A230" s="1" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="231">
       <c r="A231" s="1" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="232">
       <c r="A232" s="1" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="233">
       <c r="A233" s="1" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="234">
       <c r="A234" s="7" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="235">
       <c r="A235" s="7" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="236">
       <c r="A236" s="1" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="237">
       <c r="A237" s="1" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="238">
       <c r="A238" s="1" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="239">
       <c r="A239" s="1" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="240">
       <c r="A240" s="1" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="241">
       <c r="A241" s="1" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="242">
       <c r="A242" s="1" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="243">
       <c r="A243" s="7" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="244">
       <c r="A244" s="7" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="245">
       <c r="A245" s="7" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="246">
       <c r="A246" s="7" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="247">
       <c r="A247" s="7" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="248">
       <c r="A248" s="7" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="249">
       <c r="A249" s="7" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="250">
       <c r="A250" s="7" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="251">
-      <c r="A251" s="1" t="s">
-        <v>265</v>
+        <v>267</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="251">
+      <c r="A251" s="4" t="s">
+        <v>268</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="252">
       <c r="A252" s="1" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="253">
-      <c r="A253" s="9" t="s">
-        <v>267</v>
+      <c r="A253" s="10" t="s">
+        <v>270</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="254">
-      <c r="A254" s="9" t="s">
-        <v>268</v>
+      <c r="A254" s="10" t="s">
+        <v>271</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="255">
-      <c r="A255" s="9" t="s">
-        <v>269</v>
+      <c r="A255" s="10" t="s">
+        <v>272</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="256">
-      <c r="A256" s="9" t="s">
-        <v>270</v>
+      <c r="A256" s="10" t="s">
+        <v>273</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="257">
-      <c r="A257" s="9" t="s">
-        <v>271</v>
+      <c r="A257" s="10" t="s">
+        <v>274</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="258">
-      <c r="A258" s="9" t="s">
-        <v>272</v>
+      <c r="A258" s="10" t="s">
+        <v>275</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="259">
-      <c r="A259" s="9" t="s">
-        <v>273</v>
+      <c r="A259" s="10" t="s">
+        <v>276</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="260">
-      <c r="A260" s="9" t="s">
-        <v>274</v>
+      <c r="A260" s="10" t="s">
+        <v>277</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="261">
-      <c r="A261" s="9" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="262">
-      <c r="A262" s="1" t="s">
-        <v>276</v>
+      <c r="A261" s="10" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="262">
+      <c r="A262" s="4" t="s">
+        <v>279</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated to reflect progress.
git-svn-id: https://subversion.ucar.edu/ncldev/ncarg/branches/NCL_6_0_0@11728 10fe2890-8a40-4696-8b1d-7ccbb19c398e
</commit_message>
<xml_diff>
--- a/ni/src/ncl/NclSrcList.xlsx
+++ b/ni/src/ncl/NclSrcList.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="288">
   <si>
     <r>
       <t xml:space="preserve">Dave</t>
@@ -270,6 +270,9 @@
     <t>NclCCM.c</t>
   </si>
   <si>
+    <t>Review by someone with CCM expertise?</t>
+  </si>
+  <si>
     <t>NclCCM.h</t>
   </si>
   <si>
@@ -495,6 +498,9 @@
     <t>OpsFuncs.c</t>
   </si>
   <si>
+    <t>Need to review this with others: _NclBuildArray suggests changes, but these propagate outwards; </t>
+  </si>
+  <si>
     <t>OpsFuncs.h</t>
   </si>
   <si>
@@ -510,9 +516,15 @@
     <t>SrcTree.c</t>
   </si>
   <si>
+    <t>see SrcTree.h</t>
+  </si>
+  <si>
     <t>SrcTree.h</t>
   </si>
   <si>
+    <t>Make NclDimSizeListNode.size field into ng_size_t</t>
+  </si>
+  <si>
     <t>Symbol.c</t>
   </si>
   <si>
@@ -591,6 +603,9 @@
     <t>VarSupport.c</t>
   </si>
   <si>
+    <t>Minor modifications to local loop variables.</t>
+  </si>
+  <si>
     <t>VarSupport.h</t>
   </si>
   <si>
@@ -612,6 +627,9 @@
     <t>craybin.c</t>
   </si>
   <si>
+    <t>Needs to be reviewed in conjunction with NclCCM.c</t>
+  </si>
+  <si>
     <t>ctoiee.c</t>
   </si>
   <si>
@@ -786,7 +804,13 @@
     <t>javaAddFuncs.c</t>
   </si>
   <si>
+    <t>No changes required (Wei fixed previously?).</t>
+  </si>
+  <si>
     <t>javaAddProto.c</t>
+  </si>
+  <si>
+    <t>Changed type of unused var “dimsizes”; anticipated for future use? (code mimics AddBuiltIns.c)</t>
   </si>
   <si>
     <t>jma_3_gtb.h</t>
@@ -992,7 +1016,7 @@
       <u val="single"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1035,6 +1059,12 @@
         <bgColor rgb="00993300"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFFFFF"/>
+        <bgColor rgb="00FFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border diagonalDown="false" diagonalUp="false">
@@ -1074,7 +1104,7 @@
       <protection hidden="false" locked="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="20"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="5" numFmtId="165" xfId="20"/>
@@ -1086,6 +1116,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="6" fontId="4" numFmtId="165" xfId="20"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="20"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="7" fontId="4" numFmtId="165" xfId="20"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="8" fontId="4" numFmtId="165" xfId="20"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -1315,6 +1346,15 @@
       <c r="A13" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="B13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="14">
       <c r="A14" s="4" t="s">
@@ -1511,9 +1551,18 @@
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="32">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="32">
       <c r="A32" s="1" t="s">
         <v>43</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="33">
@@ -1665,15 +1714,27 @@
       <c r="A48" s="9" t="s">
         <v>62</v>
       </c>
+      <c r="C48" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="49">
       <c r="A49" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D49" s="1" t="s">
         <v>63</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="50">
       <c r="A50" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>6</v>
@@ -1687,7 +1748,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="51">
       <c r="A51" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>6</v>
@@ -1701,7 +1762,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="52">
       <c r="A52" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>6</v>
@@ -1715,7 +1776,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="53">
       <c r="A53" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>6</v>
@@ -1729,180 +1790,180 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="54">
       <c r="A54" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="55">
       <c r="A55" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="56">
       <c r="A56" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="57">
       <c r="A57" s="7" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="58">
       <c r="A58" s="7" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="59">
       <c r="A59" s="7" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="60">
       <c r="A60" s="7" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="61">
       <c r="A61" s="7" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="62">
       <c r="A62" s="7" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="63">
       <c r="A63" s="7" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="64">
       <c r="A64" s="7" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="65">
       <c r="A65" s="7" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="66">
       <c r="A66" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="67">
       <c r="A67" s="7" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="68">
       <c r="A68" s="10" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="69">
       <c r="A69" s="10" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="70">
       <c r="A70" s="10" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="71">
       <c r="A71" s="7" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="72">
       <c r="A72" s="7" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="73">
       <c r="A73" s="7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="74">
       <c r="A74" s="7" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="75">
       <c r="A75" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="76">
       <c r="A76" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="77">
       <c r="A77" s="7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="78">
       <c r="A78" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="79">
       <c r="A79" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="80">
       <c r="A80" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="81">
       <c r="A81" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="82">
       <c r="A82" s="7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="83">
       <c r="A83" s="7" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="84">
       <c r="A84" s="7" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="85">
       <c r="A85" s="7" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="86">
       <c r="A86" s="7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="87">
       <c r="A87" s="7" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="88">
       <c r="A88" s="4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>22</v>
@@ -1911,12 +1972,12 @@
         <v>7</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="89">
       <c r="A89" s="4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>22</v>
@@ -1925,12 +1986,12 @@
         <v>7</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="90">
       <c r="A90" s="4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>6</v>
@@ -1944,862 +2005,1459 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="91">
       <c r="A91" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="92">
       <c r="A92" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="93">
       <c r="A93" s="10" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="94">
       <c r="A94" s="10" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="95">
       <c r="A95" s="10" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="96">
       <c r="A96" s="10" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="97">
       <c r="A97" s="10" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="98">
       <c r="A98" s="10" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="99">
       <c r="A99" s="10" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="100">
       <c r="A100" s="10" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="101">
       <c r="A101" s="10" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="102">
       <c r="A102" s="10" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="103">
       <c r="A103" s="10" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="104">
       <c r="A104" s="10" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="105">
       <c r="A105" s="10" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="106">
       <c r="A106" s="10" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="107">
       <c r="A107" s="10" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="108">
       <c r="A108" s="10" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="109">
       <c r="A109" s="10" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="110">
       <c r="A110" s="10" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="111">
       <c r="A111" s="10" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="112">
       <c r="A112" s="10" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="113">
       <c r="A113" s="10" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="114">
       <c r="A114" s="10" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="115">
       <c r="A115" s="10" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="116">
       <c r="A116" s="10" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="117">
       <c r="A117" s="10" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="118">
       <c r="A118" s="7" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="119">
       <c r="A119" s="7" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="120">
       <c r="A120" s="4" t="s">
-        <v>137</v>
+        <v>138</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>139</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="121">
       <c r="A121" s="4" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="122">
       <c r="A122" s="4" t="s">
-        <v>139</v>
+        <v>141</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="123">
       <c r="A123" s="4" t="s">
-        <v>140</v>
+        <v>142</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D123" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="124">
       <c r="A124" s="4" t="s">
-        <v>141</v>
+        <v>143</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="125">
       <c r="A125" s="4" t="s">
-        <v>142</v>
+        <v>144</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>145</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="126">
       <c r="A126" s="4" t="s">
-        <v>143</v>
+        <v>146</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>147</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="127">
       <c r="A127" s="7" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="128">
       <c r="A128" s="7" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="129">
       <c r="A129" s="7" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="130">
       <c r="A130" s="7" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="131">
       <c r="A131" s="7" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="132">
       <c r="A132" s="7" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="133">
       <c r="A133" s="7" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="134">
       <c r="A134" s="7" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="135">
       <c r="A135" s="7" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="136">
       <c r="A136" s="7" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="137">
       <c r="A137" s="7" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="138">
       <c r="A138" s="7" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="139">
       <c r="A139" s="7" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="140">
       <c r="A140" s="7" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="141">
       <c r="A141" s="7" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="142">
       <c r="A142" s="7" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="143">
       <c r="A143" s="7" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="144">
       <c r="A144" s="7" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="145">
       <c r="A145" s="7" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="146">
       <c r="A146" s="7" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="147">
       <c r="A147" s="7" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="148">
       <c r="A148" s="7" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="149">
       <c r="A149" s="7" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="150">
       <c r="A150" s="7" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="151">
       <c r="A151" s="7" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="152">
       <c r="A152" s="4" t="s">
-        <v>169</v>
+        <v>173</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D152" s="1" t="s">
+        <v>174</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="153">
       <c r="A153" s="4" t="s">
-        <v>170</v>
+        <v>175</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D153" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="154">
       <c r="A154" s="1" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="155">
       <c r="A155" s="4" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="156">
       <c r="A156" s="1" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="157">
       <c r="A157" s="4" t="s">
-        <v>174</v>
+        <v>179</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D157" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="158">
       <c r="A158" s="4" t="s">
-        <v>175</v>
+        <v>180</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D158" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="159">
-      <c r="A159" s="4" t="s">
-        <v>176</v>
+      <c r="A159" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D159" s="1" t="s">
+        <v>182</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="160">
       <c r="A160" s="4" t="s">
-        <v>177</v>
+        <v>183</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C160" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D160" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="161">
       <c r="A161" s="1" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="162">
       <c r="A162" s="4" t="s">
-        <v>179</v>
+        <v>185</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C162" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D162" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="163">
       <c r="A163" s="4" t="s">
-        <v>180</v>
+        <v>186</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C163" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D163" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="164">
       <c r="A164" s="4" t="s">
-        <v>181</v>
+        <v>187</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D164" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="165">
       <c r="A165" s="1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="166">
+        <v>188</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="166">
       <c r="A166" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="167">
+        <v>189</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C166" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D166" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="167">
       <c r="A167" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="168">
+        <v>190</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C167" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D167" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="168">
       <c r="A168" s="1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="169">
+        <v>191</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D168" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="169">
       <c r="A169" s="1" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="170">
+        <v>192</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C169" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D169" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="170">
       <c r="A170" s="1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="171">
+        <v>193</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C170" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D170" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="171">
       <c r="A171" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="172">
+        <v>194</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C171" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D171" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="172">
       <c r="A172" s="1" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="173">
+        <v>195</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C172" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D172" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="173">
       <c r="A173" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="174">
+        <v>196</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C173" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D173" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="174">
       <c r="A174" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="175">
+        <v>197</v>
+      </c>
+      <c r="B174" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C174" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D174" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="175">
       <c r="A175" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="176">
+        <v>198</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C175" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D175" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="176">
       <c r="A176" s="1" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="177">
+        <v>199</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C176" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D176" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="177">
       <c r="A177" s="1" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="178">
+        <v>200</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C177" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D177" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="178">
       <c r="A178" s="1" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="179">
+        <v>201</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C178" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D178" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="179">
       <c r="A179" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="180">
+        <v>202</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C179" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D179" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="180">
       <c r="A180" s="1" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="181">
+        <v>203</v>
+      </c>
+      <c r="B180" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C180" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D180" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="181">
       <c r="A181" s="1" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="182">
+        <v>204</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C181" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D181" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="182">
       <c r="A182" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="183">
+        <v>205</v>
+      </c>
+      <c r="B182" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C182" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D182" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="183">
       <c r="A183" s="1" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="184">
+        <v>206</v>
+      </c>
+      <c r="B183" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C183" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D183" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="184">
       <c r="A184" s="1" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="185">
+        <v>207</v>
+      </c>
+      <c r="B184" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C184" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D184" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="185">
       <c r="A185" s="1" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="186">
+        <v>208</v>
+      </c>
+      <c r="B185" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C185" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D185" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="186">
       <c r="A186" s="1" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="187">
+        <v>209</v>
+      </c>
+      <c r="B186" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C186" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D186" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="187">
       <c r="A187" s="1" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="188">
+        <v>210</v>
+      </c>
+      <c r="B187" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C187" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D187" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="188">
       <c r="A188" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="189">
+        <v>211</v>
+      </c>
+      <c r="B188" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C188" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D188" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="189">
       <c r="A189" s="1" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="190">
+        <v>212</v>
+      </c>
+      <c r="B189" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C189" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D189" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="190">
       <c r="A190" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="191">
+        <v>213</v>
+      </c>
+      <c r="B190" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C190" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D190" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="191">
       <c r="A191" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="192">
+        <v>214</v>
+      </c>
+      <c r="B191" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C191" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D191" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="192">
       <c r="A192" s="1" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="193">
+        <v>215</v>
+      </c>
+      <c r="B192" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C192" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D192" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="193">
       <c r="A193" s="1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="194">
+        <v>216</v>
+      </c>
+      <c r="B193" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C193" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D193" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="194">
       <c r="A194" s="1" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="195">
+        <v>217</v>
+      </c>
+      <c r="B194" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C194" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D194" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="195">
       <c r="A195" s="1" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="196">
+        <v>218</v>
+      </c>
+      <c r="B195" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C195" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D195" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="196">
       <c r="A196" s="1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="197">
+        <v>219</v>
+      </c>
+      <c r="B196" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C196" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D196" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="197">
       <c r="A197" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="198">
+        <v>220</v>
+      </c>
+      <c r="B197" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C197" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D197" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="198">
       <c r="A198" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="199">
+        <v>221</v>
+      </c>
+      <c r="B198" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C198" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D198" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="199">
       <c r="A199" s="1" t="s">
-        <v>216</v>
+        <v>222</v>
+      </c>
+      <c r="B199" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C199" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D199" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="200">
       <c r="A200" s="4" t="s">
-        <v>217</v>
+        <v>223</v>
+      </c>
+      <c r="B200" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C200" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D200" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="201">
       <c r="A201" s="4" t="s">
-        <v>218</v>
+        <v>224</v>
+      </c>
+      <c r="B201" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C201" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D201" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="202">
       <c r="A202" s="4" t="s">
-        <v>219</v>
+        <v>225</v>
+      </c>
+      <c r="B202" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C202" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D202" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="203">
       <c r="A203" s="1" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="204">
       <c r="A204" s="1" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="205">
       <c r="A205" s="1" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="206">
       <c r="A206" s="1" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="207">
       <c r="A207" s="1" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="208">
       <c r="A208" s="1" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="209">
       <c r="A209" s="1" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="210">
       <c r="A210" s="1" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="211">
       <c r="A211" s="1" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="212">
       <c r="A212" s="1" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="213">
       <c r="A213" s="1" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="214">
       <c r="A214" s="1" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="215">
       <c r="A215" s="1" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="216">
       <c r="A216" s="4" t="s">
-        <v>233</v>
+        <v>239</v>
+      </c>
+      <c r="B216" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C216" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D216" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="217">
       <c r="A217" s="4" t="s">
-        <v>234</v>
+        <v>240</v>
+      </c>
+      <c r="B217" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C217" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D217" s="1" t="s">
+        <v>241</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="218">
       <c r="A218" s="4" t="s">
-        <v>235</v>
+        <v>242</v>
+      </c>
+      <c r="B218" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C218" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D218" s="1" t="s">
+        <v>243</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="219">
       <c r="A219" s="1" t="s">
-        <v>236</v>
+        <v>244</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="220">
       <c r="A220" s="1" t="s">
-        <v>237</v>
+        <v>245</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="221">
       <c r="A221" s="1" t="s">
-        <v>238</v>
+        <v>246</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="222">
       <c r="A222" s="1" t="s">
-        <v>239</v>
+        <v>247</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="223">
       <c r="A223" s="1" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="224">
+        <v>248</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="224">
       <c r="A224" s="1" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="225">
+        <v>249</v>
+      </c>
+      <c r="B224" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C224" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D224" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="225">
       <c r="A225" s="1" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="226">
+        <v>250</v>
+      </c>
+      <c r="B225" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C225" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D225" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="226">
       <c r="A226" s="1" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="227">
+        <v>251</v>
+      </c>
+      <c r="B226" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C226" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D226" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="227">
       <c r="A227" s="1" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="228">
+        <v>252</v>
+      </c>
+      <c r="B227" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C227" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D227" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="228">
       <c r="A228" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="229">
+        <v>253</v>
+      </c>
+      <c r="B228" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C228" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D228" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="229">
       <c r="A229" s="1" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="230">
+        <v>254</v>
+      </c>
+      <c r="B229" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C229" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D229" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="230">
       <c r="A230" s="1" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="231">
+        <v>255</v>
+      </c>
+      <c r="B230" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C230" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D230" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="231">
       <c r="A231" s="1" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="232">
+        <v>256</v>
+      </c>
+      <c r="B231" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C231" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D231" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="232">
       <c r="A232" s="1" t="s">
-        <v>249</v>
+        <v>257</v>
+      </c>
+      <c r="B232" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C232" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D232" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="233">
       <c r="A233" s="1" t="s">
-        <v>250</v>
+        <v>258</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="234">
       <c r="A234" s="7" t="s">
-        <v>251</v>
+        <v>259</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="235">
       <c r="A235" s="7" t="s">
-        <v>252</v>
+        <v>260</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="236">
       <c r="A236" s="1" t="s">
-        <v>253</v>
+        <v>261</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="237">
       <c r="A237" s="1" t="s">
-        <v>254</v>
+        <v>262</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="238">
       <c r="A238" s="1" t="s">
-        <v>255</v>
+        <v>263</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="239">
       <c r="A239" s="1" t="s">
-        <v>256</v>
+        <v>264</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="240">
       <c r="A240" s="1" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="241">
       <c r="A241" s="1" t="s">
-        <v>258</v>
+        <v>266</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="242">
       <c r="A242" s="1" t="s">
-        <v>259</v>
+        <v>267</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="243">
       <c r="A243" s="7" t="s">
-        <v>260</v>
+        <v>268</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="244">
       <c r="A244" s="7" t="s">
-        <v>261</v>
+        <v>269</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="245">
       <c r="A245" s="7" t="s">
-        <v>262</v>
+        <v>270</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="246">
       <c r="A246" s="7" t="s">
-        <v>263</v>
+        <v>271</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="247">
       <c r="A247" s="7" t="s">
-        <v>264</v>
+        <v>272</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="248">
       <c r="A248" s="7" t="s">
-        <v>265</v>
+        <v>273</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="249">
       <c r="A249" s="7" t="s">
-        <v>266</v>
+        <v>274</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="250">
       <c r="A250" s="7" t="s">
-        <v>267</v>
+        <v>275</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="251">
       <c r="A251" s="4" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="252">
+        <v>276</v>
+      </c>
+      <c r="B251" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C251" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D251" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="252">
       <c r="A252" s="1" t="s">
-        <v>269</v>
+        <v>277</v>
+      </c>
+      <c r="B252" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C252" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D252" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="253">
       <c r="A253" s="10" t="s">
-        <v>270</v>
+        <v>278</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="254">
       <c r="A254" s="10" t="s">
-        <v>271</v>
+        <v>279</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="255">
       <c r="A255" s="10" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="256">
       <c r="A256" s="10" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="257">
       <c r="A257" s="10" t="s">
-        <v>274</v>
+        <v>282</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="258">
       <c r="A258" s="10" t="s">
-        <v>275</v>
+        <v>283</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="259">
       <c r="A259" s="10" t="s">
-        <v>276</v>
+        <v>284</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="260">
       <c r="A260" s="10" t="s">
-        <v>277</v>
+        <v>285</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="261">
       <c r="A261" s="10" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="262">
       <c r="A262" s="4" t="s">
-        <v>279</v>
+        <v>287</v>
+      </c>
+      <c r="B262" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C262" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D262" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated to show latest progress.
git-svn-id: https://subversion.ucar.edu/ncldev/ncarg/branches/NCL_6_0_0@11735 10fe2890-8a40-4696-8b1d-7ccbb19c398e
</commit_message>
<xml_diff>
--- a/ni/src/ncl/NclSrcList.xlsx
+++ b/ni/src/ncl/NclSrcList.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="289">
   <si>
     <r>
       <t xml:space="preserve">Dave</t>
@@ -164,6 +164,9 @@
   </si>
   <si>
     <t>HLUFunctions.c</t>
+  </si>
+  <si>
+    <t>Many changes, mostly to promote variable “total” throughout. _NclAddToOverlay2() severely dysfunctional!</t>
   </si>
   <si>
     <t>HLUFunctions.h</t>
@@ -1337,9 +1340,18 @@
         <v>18</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="12">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="12">
       <c r="A12" s="6" t="s">
         <v>19</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="13">
@@ -1433,29 +1445,65 @@
         <v>30</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="21">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="21">
       <c r="A21" s="6" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="22">
+      <c r="B21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="22">
       <c r="A22" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="23">
+        <v>33</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="23">
       <c r="A23" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="24">
+        <v>34</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="24">
       <c r="A24" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="25">
       <c r="A25" s="8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>6</v>
@@ -1469,7 +1517,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="26">
       <c r="A26" s="8" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>6</v>
@@ -1483,7 +1531,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="27">
       <c r="A27" s="8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>6</v>
@@ -1497,7 +1545,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="28">
       <c r="A28" s="8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>6</v>
@@ -1511,7 +1559,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="29">
       <c r="A29" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>6</v>
@@ -1525,7 +1573,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="30">
       <c r="A30" s="8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>22</v>
@@ -1534,12 +1582,12 @@
         <v>7</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="31">
       <c r="A31" s="8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>6</v>
@@ -1553,7 +1601,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="32">
       <c r="A32" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>6</v>
@@ -1567,37 +1615,37 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="33">
       <c r="A33" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="34">
       <c r="A34" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="35">
       <c r="A35" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="36">
       <c r="A36" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="37">
       <c r="A37" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="38">
       <c r="A38" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="39">
       <c r="A39" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>6</v>
@@ -1611,12 +1659,12 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="40">
       <c r="A40" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="41">
       <c r="A41" s="8" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>6</v>
@@ -1630,7 +1678,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="42">
       <c r="A42" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>22</v>
@@ -1639,12 +1687,12 @@
         <v>7</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="43">
       <c r="A43" s="8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>6</v>
@@ -1656,10 +1704,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="44">
       <c r="A44" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>7</v>
@@ -1670,7 +1718,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="45">
       <c r="A45" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>6</v>
@@ -1679,12 +1727,12 @@
         <v>7</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="46">
       <c r="A46" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>6</v>
@@ -1698,7 +1746,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="47">
       <c r="A47" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>6</v>
@@ -1712,29 +1760,29 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="48">
       <c r="A48" s="9" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="49">
       <c r="A49" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D49" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="50">
       <c r="A50" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>6</v>
@@ -1748,7 +1796,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="51">
       <c r="A51" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>6</v>
@@ -1762,7 +1810,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="52">
       <c r="A52" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>6</v>
@@ -1776,7 +1824,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="53">
       <c r="A53" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>6</v>
@@ -1790,180 +1838,180 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="54">
       <c r="A54" s="7" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="55">
       <c r="A55" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="56">
       <c r="A56" s="7" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="57">
       <c r="A57" s="7" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="58">
       <c r="A58" s="7" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="59">
       <c r="A59" s="7" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="60">
       <c r="A60" s="7" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="61">
       <c r="A61" s="7" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="62">
       <c r="A62" s="7" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="63">
       <c r="A63" s="7" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="64">
       <c r="A64" s="7" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="65">
       <c r="A65" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="66">
       <c r="A66" s="7" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="67">
       <c r="A67" s="7" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="68">
       <c r="A68" s="10" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="69">
       <c r="A69" s="10" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="70">
       <c r="A70" s="10" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="71">
       <c r="A71" s="7" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="72">
       <c r="A72" s="7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="73">
       <c r="A73" s="7" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="74">
       <c r="A74" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="75">
       <c r="A75" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="76">
       <c r="A76" s="7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="77">
       <c r="A77" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="78">
       <c r="A78" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="79">
       <c r="A79" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="80">
       <c r="A80" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="81">
       <c r="A81" s="7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="82">
       <c r="A82" s="7" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="83">
       <c r="A83" s="7" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="84">
       <c r="A84" s="7" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="85">
       <c r="A85" s="7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="86">
       <c r="A86" s="7" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="87">
       <c r="A87" s="7" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="88">
       <c r="A88" s="4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>22</v>
@@ -1972,12 +2020,12 @@
         <v>7</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="89">
       <c r="A89" s="4" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>22</v>
@@ -1986,12 +2034,12 @@
         <v>7</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="90">
       <c r="A90" s="4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>6</v>
@@ -2005,168 +2053,168 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="91">
       <c r="A91" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="92">
       <c r="A92" s="10" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="93">
       <c r="A93" s="10" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="94">
       <c r="A94" s="10" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="95">
       <c r="A95" s="10" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="96">
       <c r="A96" s="10" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="97">
       <c r="A97" s="10" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="98">
       <c r="A98" s="10" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="99">
       <c r="A99" s="10" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="100">
       <c r="A100" s="10" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="101">
       <c r="A101" s="10" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="102">
       <c r="A102" s="10" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="103">
       <c r="A103" s="10" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="104">
       <c r="A104" s="10" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="105">
       <c r="A105" s="10" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="106">
       <c r="A106" s="10" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="107">
       <c r="A107" s="10" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="108">
       <c r="A108" s="10" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="109">
       <c r="A109" s="10" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="110">
       <c r="A110" s="10" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="111">
       <c r="A111" s="10" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="112">
       <c r="A112" s="10" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="113">
       <c r="A113" s="10" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="114">
       <c r="A114" s="10" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="115">
       <c r="A115" s="10" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="116">
       <c r="A116" s="10" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="117">
       <c r="A117" s="10" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="118">
       <c r="A118" s="7" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="119">
       <c r="A119" s="7" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="120">
       <c r="A120" s="4" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="121">
       <c r="A121" s="4" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="122">
       <c r="A122" s="4" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>6</v>
@@ -2180,7 +2228,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="123">
       <c r="A123" s="4" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>6</v>
@@ -2194,7 +2242,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="124">
       <c r="A124" s="4" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>6</v>
@@ -2208,21 +2256,21 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="125">
       <c r="A125" s="4" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C125" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="126">
       <c r="A126" s="4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B126" s="1" t="s">
         <v>22</v>
@@ -2231,137 +2279,137 @@
         <v>7</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="127">
       <c r="A127" s="7" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="128">
       <c r="A128" s="7" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="129">
       <c r="A129" s="7" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="130">
       <c r="A130" s="7" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="131">
       <c r="A131" s="7" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="132">
       <c r="A132" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="133">
       <c r="A133" s="7" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="134">
       <c r="A134" s="7" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="135">
       <c r="A135" s="7" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="136">
       <c r="A136" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="137">
       <c r="A137" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="138">
       <c r="A138" s="7" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="139">
       <c r="A139" s="7" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="140">
       <c r="A140" s="7" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="141">
       <c r="A141" s="7" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="142">
       <c r="A142" s="7" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="143">
       <c r="A143" s="7" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="144">
       <c r="A144" s="7" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="145">
       <c r="A145" s="7" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="146">
       <c r="A146" s="7" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="147">
       <c r="A147" s="7" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="148">
       <c r="A148" s="7" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="149">
       <c r="A149" s="7" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="150">
       <c r="A150" s="7" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="151">
       <c r="A151" s="7" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="152">
       <c r="A152" s="4" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B152" s="1" t="s">
         <v>22</v>
@@ -2370,12 +2418,12 @@
         <v>7</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="153">
       <c r="A153" s="4" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B153" s="1" t="s">
         <v>6</v>
@@ -2389,22 +2437,22 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="154">
       <c r="A154" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="155">
       <c r="A155" s="4" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="156">
       <c r="A156" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="157">
       <c r="A157" s="4" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B157" s="1" t="s">
         <v>6</v>
@@ -2418,7 +2466,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="158">
       <c r="A158" s="4" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B158" s="1" t="s">
         <v>6</v>
@@ -2432,18 +2480,18 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="159">
       <c r="A159" s="11" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C159" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="160">
       <c r="A160" s="4" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B160" s="1" t="s">
         <v>6</v>
@@ -2457,12 +2505,12 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="161">
       <c r="A161" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="162">
       <c r="A162" s="4" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B162" s="1" t="s">
         <v>6</v>
@@ -2476,7 +2524,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="163">
       <c r="A163" s="4" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B163" s="1" t="s">
         <v>6</v>
@@ -2490,7 +2538,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="164">
       <c r="A164" s="4" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B164" s="1" t="s">
         <v>6</v>
@@ -2504,12 +2552,12 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="165">
       <c r="A165" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="166">
       <c r="A166" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B166" s="1" t="s">
         <v>6</v>
@@ -2523,7 +2571,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="167">
       <c r="A167" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B167" s="1" t="s">
         <v>6</v>
@@ -2537,7 +2585,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="168">
       <c r="A168" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B168" s="1" t="s">
         <v>6</v>
@@ -2551,7 +2599,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="169">
       <c r="A169" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B169" s="1" t="s">
         <v>6</v>
@@ -2565,7 +2613,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="170">
       <c r="A170" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B170" s="1" t="s">
         <v>6</v>
@@ -2579,7 +2627,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="171">
       <c r="A171" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B171" s="1" t="s">
         <v>6</v>
@@ -2593,7 +2641,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="172">
       <c r="A172" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B172" s="1" t="s">
         <v>6</v>
@@ -2607,7 +2655,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="173">
       <c r="A173" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B173" s="1" t="s">
         <v>6</v>
@@ -2621,7 +2669,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="174">
       <c r="A174" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B174" s="1" t="s">
         <v>6</v>
@@ -2635,7 +2683,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="175">
       <c r="A175" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B175" s="1" t="s">
         <v>6</v>
@@ -2649,7 +2697,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="176">
       <c r="A176" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B176" s="1" t="s">
         <v>6</v>
@@ -2663,7 +2711,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="177">
       <c r="A177" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B177" s="1" t="s">
         <v>6</v>
@@ -2677,7 +2725,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="178">
       <c r="A178" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B178" s="1" t="s">
         <v>6</v>
@@ -2691,7 +2739,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="179">
       <c r="A179" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B179" s="1" t="s">
         <v>6</v>
@@ -2705,7 +2753,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="180">
       <c r="A180" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B180" s="1" t="s">
         <v>6</v>
@@ -2719,7 +2767,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="181">
       <c r="A181" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B181" s="1" t="s">
         <v>6</v>
@@ -2733,7 +2781,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="182">
       <c r="A182" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B182" s="1" t="s">
         <v>6</v>
@@ -2747,7 +2795,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="183">
       <c r="A183" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B183" s="1" t="s">
         <v>6</v>
@@ -2761,7 +2809,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="184">
       <c r="A184" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B184" s="1" t="s">
         <v>6</v>
@@ -2775,7 +2823,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="185">
       <c r="A185" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B185" s="1" t="s">
         <v>6</v>
@@ -2789,7 +2837,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="186">
       <c r="A186" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B186" s="1" t="s">
         <v>6</v>
@@ -2803,7 +2851,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="187">
       <c r="A187" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B187" s="1" t="s">
         <v>6</v>
@@ -2817,7 +2865,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="188">
       <c r="A188" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B188" s="1" t="s">
         <v>6</v>
@@ -2831,7 +2879,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="189">
       <c r="A189" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B189" s="1" t="s">
         <v>6</v>
@@ -2845,7 +2893,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="190">
       <c r="A190" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B190" s="1" t="s">
         <v>6</v>
@@ -2859,7 +2907,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="191">
       <c r="A191" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B191" s="1" t="s">
         <v>6</v>
@@ -2873,7 +2921,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="192">
       <c r="A192" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B192" s="1" t="s">
         <v>6</v>
@@ -2887,7 +2935,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="193">
       <c r="A193" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B193" s="1" t="s">
         <v>6</v>
@@ -2901,7 +2949,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="194">
       <c r="A194" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B194" s="1" t="s">
         <v>6</v>
@@ -2915,7 +2963,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="195">
       <c r="A195" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B195" s="1" t="s">
         <v>6</v>
@@ -2929,7 +2977,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="196">
       <c r="A196" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B196" s="1" t="s">
         <v>6</v>
@@ -2943,7 +2991,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="197">
       <c r="A197" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B197" s="1" t="s">
         <v>6</v>
@@ -2957,7 +3005,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="198">
       <c r="A198" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B198" s="1" t="s">
         <v>6</v>
@@ -2971,7 +3019,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="199">
       <c r="A199" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B199" s="1" t="s">
         <v>6</v>
@@ -2985,7 +3033,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="200">
       <c r="A200" s="4" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B200" s="1" t="s">
         <v>6</v>
@@ -2999,7 +3047,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="201">
       <c r="A201" s="4" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B201" s="1" t="s">
         <v>6</v>
@@ -3013,7 +3061,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="202">
       <c r="A202" s="4" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B202" s="1" t="s">
         <v>6</v>
@@ -3027,72 +3075,72 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="203">
       <c r="A203" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="204">
       <c r="A204" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="205">
       <c r="A205" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="206">
       <c r="A206" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="207">
       <c r="A207" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="208">
       <c r="A208" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="209">
       <c r="A209" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="210">
       <c r="A210" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="211">
       <c r="A211" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="212">
       <c r="A212" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="213">
       <c r="A213" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="214">
       <c r="A214" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="215">
       <c r="A215" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="216">
       <c r="A216" s="4" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B216" s="1" t="s">
         <v>6</v>
@@ -3106,7 +3154,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="217">
       <c r="A217" s="4" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B217" s="1" t="s">
         <v>6</v>
@@ -3115,12 +3163,12 @@
         <v>7</v>
       </c>
       <c r="D217" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="218">
       <c r="A218" s="4" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B218" s="1" t="s">
         <v>22</v>
@@ -3129,37 +3177,37 @@
         <v>7</v>
       </c>
       <c r="D218" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="219">
       <c r="A219" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="220">
       <c r="A220" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="221">
       <c r="A221" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="222">
       <c r="A222" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="223">
       <c r="A223" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="224">
       <c r="A224" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B224" s="1" t="s">
         <v>6</v>
@@ -3173,7 +3221,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="225">
       <c r="A225" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B225" s="1" t="s">
         <v>6</v>
@@ -3187,7 +3235,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="226">
       <c r="A226" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B226" s="1" t="s">
         <v>6</v>
@@ -3201,7 +3249,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="227">
       <c r="A227" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B227" s="1" t="s">
         <v>6</v>
@@ -3215,7 +3263,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="228">
       <c r="A228" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B228" s="1" t="s">
         <v>6</v>
@@ -3229,7 +3277,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="229">
       <c r="A229" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B229" s="1" t="s">
         <v>6</v>
@@ -3243,7 +3291,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="230">
       <c r="A230" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B230" s="1" t="s">
         <v>6</v>
@@ -3257,7 +3305,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="231">
       <c r="A231" s="1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B231" s="1" t="s">
         <v>6</v>
@@ -3271,7 +3319,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="232">
       <c r="A232" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B232" s="1" t="s">
         <v>6</v>
@@ -3285,97 +3333,97 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="233">
       <c r="A233" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="234">
       <c r="A234" s="7" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="235">
       <c r="A235" s="7" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="236">
       <c r="A236" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="237">
       <c r="A237" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="238">
       <c r="A238" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="239">
       <c r="A239" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="240">
       <c r="A240" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="241">
       <c r="A241" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="242">
       <c r="A242" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="243">
       <c r="A243" s="7" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="244">
       <c r="A244" s="7" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="245">
       <c r="A245" s="7" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="246">
       <c r="A246" s="7" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="247">
       <c r="A247" s="7" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="248">
       <c r="A248" s="7" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="249">
       <c r="A249" s="7" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="250">
       <c r="A250" s="7" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="251">
       <c r="A251" s="4" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B251" s="1" t="s">
         <v>6</v>
@@ -3389,7 +3437,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="252">
       <c r="A252" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B252" s="1" t="s">
         <v>6</v>
@@ -3403,52 +3451,52 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="253">
       <c r="A253" s="10" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="254">
       <c r="A254" s="10" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="255">
       <c r="A255" s="10" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="256">
       <c r="A256" s="10" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="257">
       <c r="A257" s="10" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="258">
       <c r="A258" s="10" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="259">
       <c r="A259" s="10" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="260">
       <c r="A260" s="10" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="261">
       <c r="A261" s="10" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="262">
       <c r="A262" s="4" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B262" s="1" t="s">
         <v>6</v>

</xml_diff>